<commit_message>
EPBDS-13258 Property file is not read from dependent project
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-12727/Child Project/Main.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-12727/Child Project/Main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpikus/.openl/user-workspace/DEFAULT/MessageBundle/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\EPBDS-12727\Child Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50E2C4B-AB95-8B4B-B993-65FE6F373671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D738D0-90E6-472D-AF03-9D51D345732D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="34940" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19330" yWindow="6220" windowWidth="18390" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
@@ -20,9 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -139,16 +137,16 @@
     <t>de</t>
   </si>
   <si>
-    <t>say.hello</t>
-  </si>
-  <si>
-    <t>say.hello.1</t>
-  </si>
-  <si>
-    <t>jar.say.hello</t>
-  </si>
-  <si>
-    <t>jar.say.hello.1</t>
+    <t>Hello, from Project!</t>
+  </si>
+  <si>
+    <t>Hello, from Jar!</t>
+  </si>
+  <si>
+    <t>Bonjour, Parameter!</t>
+  </si>
+  <si>
+    <t>Bonjour, from MessageBundle!</t>
   </si>
 </sst>
 </file>
@@ -202,7 +200,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -567,27 +565,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25:F26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" style="1"/>
-    <col min="5" max="6" width="26.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="15.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.90625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="26.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,7 +593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -603,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -611,7 +609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -619,7 +617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -627,7 +625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -635,7 +633,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -643,7 +641,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
@@ -651,7 +649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -659,12 +657,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
@@ -681,7 +679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
@@ -695,7 +693,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
@@ -712,7 +710,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
@@ -720,16 +718,16 @@
         <v>22</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
@@ -740,13 +738,13 @@
         <v>31</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
@@ -757,13 +755,13 @@
         <v>32</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
@@ -771,16 +769,16 @@
         <v>25</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
@@ -788,16 +786,16 @@
         <v>26</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
@@ -814,7 +812,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>